<commit_message>
fixing the mobile config kpis
</commit_message>
<xml_diff>
--- a/Projects/SINOTH/Data/Template.xlsx
+++ b/Projects/SINOTH/Data/Template.xlsx
@@ -190,7 +190,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,14 +229,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3399FF"/>
-        <bgColor rgb="FF00CCFF"/>
+        <fgColor rgb="FF99FFFF"/>
+        <bgColor rgb="FFC5F9CB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC2E8FB"/>
-        <bgColor rgb="FFC8F9D0"/>
+        <fgColor rgb="FF33FF99"/>
+        <bgColor rgb="FF66FF99"/>
       </patternFill>
     </fill>
     <fill>
@@ -265,14 +265,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FFFF"/>
-        <bgColor rgb="FFC2E8FB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF33FF99"/>
-        <bgColor rgb="FF66FF99"/>
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor rgb="FFF69ABE"/>
       </patternFill>
     </fill>
   </fills>
@@ -338,7 +332,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -375,11 +369,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,43 +421,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -499,7 +473,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -525,7 +499,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF66FF99"/>
+      <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
@@ -551,14 +525,14 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFC2E8FB"/>
+      <rgbColor rgb="FF99FFFF"/>
       <rgbColor rgb="FFC8F9D0"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99FFFF"/>
+      <rgbColor rgb="FF66FF99"/>
       <rgbColor rgb="FFF69ABE"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFF66CC"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3399FF"/>
+      <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33FF99"/>
       <rgbColor rgb="FF66CC00"/>
       <rgbColor rgb="FFFFCC00"/>
@@ -587,16 +561,16 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="6:7 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.4030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -691,31 +665,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMH7"/>
+  <dimension ref="1:7"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topRight" activeCell="A7" activeCellId="0" sqref="6:7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="55.4795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="11" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="11" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1022" min="15" style="11" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="54.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="55.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="11" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="11" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1021" min="15" style="11" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1765,7 +1739,6 @@
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13"/>
@@ -2803,7 +2776,6 @@
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
       <c r="AMG2" s="0"/>
-      <c r="AMH2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -3843,7 +3815,6 @@
       <c r="AME3" s="0"/>
       <c r="AMF3" s="0"/>
       <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -3869,14 +3840,14 @@
       <c r="K4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>29</v>
+      <c r="L4" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="M4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="14" t="s">
-        <v>27</v>
+      <c r="N4" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="O4" s="0"/>
       <c r="P4" s="0"/>
@@ -4885,37 +4856,36 @@
       <c r="AME4" s="0"/>
       <c r="AMF4" s="0"/>
       <c r="AMG4" s="0"/>
-      <c r="AMH4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="24" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="24" t="s">
+      <c r="H5" s="16"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="29" t="s">
+      <c r="M5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="N5" s="14" t="s">
         <v>27</v>
       </c>
       <c r="O5" s="0"/>
@@ -5925,77 +5895,82 @@
       <c r="AME5" s="0"/>
       <c r="AMF5" s="0"/>
       <c r="AMG5" s="0"/>
-      <c r="AMH5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+    <row r="6" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="24" t="s">
+      <c r="F6" s="18"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="28" t="s">
+      <c r="N6" s="14" t="s">
         <v>29</v>
       </c>
+      <c r="AMH6" s="25"/>
+      <c r="AMI6" s="25"/>
+      <c r="AMJ6" s="25"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
+    <row r="7" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="24" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="29" t="s">
+      <c r="L7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="28" t="s">
-        <v>27</v>
-      </c>
+      <c r="N7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="AMH7" s="25"/>
+      <c r="AMI7" s="25"/>
+      <c r="AMJ7" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6016,49 +5991,48 @@
   <dimension ref="1:8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="6:7 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="32" width="58.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="32" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="32" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="33" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="32" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="32" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="32" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="32" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="55.2091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="27" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="6.75"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="28" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="27" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+    <row r="1" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="31" t="s">
         <v>39</v>
       </c>
     </row>
@@ -6066,24 +6040,24 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="38" t="n">
+      <c r="B2" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="38" t="n">
+      <c r="C2" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="38" t="n">
+      <c r="D2" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="38" t="n">
+      <c r="E2" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
@@ -7104,127 +7078,127 @@
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="39" t="n">
+      <c r="B3" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="39" t="n">
+      <c r="C3" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="39" t="n">
+      <c r="D3" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="39" t="n">
+      <c r="E3" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="39" t="n">
+      <c r="B4" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="39" t="n">
+      <c r="C4" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="39" t="n">
+      <c r="D4" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="39" t="n">
+      <c r="E4" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
       <c r="J4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="39" t="n">
+      <c r="B5" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="39" t="n">
+      <c r="C5" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="39" t="n">
+      <c r="D5" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="39" t="n">
+      <c r="E5" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
       <c r="J5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="39" t="n">
+      <c r="B6" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="39" t="n">
+      <c r="C6" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="39" t="n">
+      <c r="D6" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="39" t="n">
+      <c r="E6" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="39" t="n">
+      <c r="B7" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="39" t="n">
+      <c r="C7" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="39" t="n">
+      <c r="D7" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="39" t="n">
+      <c r="E7" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="39" t="n">
+      <c r="B8" s="34" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -7233,10 +7207,10 @@
       <c r="D8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="33" t="s">
         <v>40</v>
       </c>
       <c r="G8" s="4" t="s">

</xml_diff>

<commit_message>
fix calc and remove general
</commit_message>
<xml_diff>
--- a/Projects/SINOTH/Data/Template.xlsx
+++ b/Projects/SINOTH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="44">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t xml:space="preserve">Main Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">candy, chocolate, gum, gummy</t>
   </si>
   <si>
     <t xml:space="preserve">ASSORTMENTS</t>
@@ -332,7 +335,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -481,6 +484,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -561,17 +568,17 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="6:7 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,26 +674,26 @@
   </sheetPr>
   <dimension ref="1:7"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A7" activeCellId="0" sqref="6:7"/>
+      <selection pane="topRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="54.1326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="55.8877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="11" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="11" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1021" min="15" style="11" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="52.780612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="11" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="11" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1021" min="15" style="11" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5933,7 +5940,7 @@
       <c r="AMI6" s="25"/>
       <c r="AMJ6" s="25"/>
     </row>
-    <row r="7" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
         <v>9</v>
       </c>
@@ -5990,21 +5997,22 @@
   </sheetPr>
   <dimension ref="1:8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="6:7 A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="27" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="6.75"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="28" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="27" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="6.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="28" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="27" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6055,7 +6063,9 @@
       <c r="F2" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="33"/>
+      <c r="G2" s="33" t="s">
+        <v>41</v>
+      </c>
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
       <c r="J2" s="0"/>
@@ -7093,7 +7103,9 @@
       <c r="F3" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="34" t="s">
+        <v>41</v>
+      </c>
       <c r="H3" s="34"/>
       <c r="I3" s="34"/>
       <c r="J3" s="0"/>
@@ -7117,7 +7129,9 @@
       <c r="F4" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="34"/>
+      <c r="G4" s="34" t="s">
+        <v>41</v>
+      </c>
       <c r="H4" s="34"/>
       <c r="I4" s="34"/>
       <c r="J4" s="0"/>
@@ -7141,7 +7155,9 @@
       <c r="F5" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="34"/>
+      <c r="G5" s="34" t="s">
+        <v>41</v>
+      </c>
       <c r="H5" s="34"/>
       <c r="I5" s="34"/>
       <c r="J5" s="0"/>
@@ -7165,7 +7181,9 @@
       <c r="F6" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="34"/>
+      <c r="G6" s="34" t="s">
+        <v>41</v>
+      </c>
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
       <c r="J6" s="0"/>
@@ -7189,38 +7207,40 @@
       <c r="F7" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="34"/>
+      <c r="G7" s="34" t="s">
+        <v>41</v>
+      </c>
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
       <c r="J7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="34" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F8" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>42</v>
+      <c r="G8" s="37" t="s">
+        <v>41</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
template update to exclude irrelevant
</commit_message>
<xml_diff>
--- a/Projects/SINOTH/Data/Template.xlsx
+++ b/Projects/SINOTH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -573,12 +573,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,18 +680,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="52.780612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="11" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="11" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1021" min="15" style="11" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="52.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="11" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="11" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1021" min="15" style="11" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5998,21 +5996,21 @@
   <dimension ref="1:8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="6.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="28" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="27" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="28" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="27" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6055,7 +6053,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="33" t="n">
         <v>0</v>
@@ -7095,7 +7093,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="34" t="n">
         <v>0</v>
@@ -7121,7 +7119,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="34" t="n">
         <v>0</v>
@@ -7147,7 +7145,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="34" t="n">
         <v>0</v>
@@ -7173,7 +7171,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="34" t="n">
         <v>0</v>
@@ -7199,7 +7197,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="34" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
adding kpis for simon
</commit_message>
<xml_diff>
--- a/Projects/SINOTH/Data/Template.xlsx
+++ b/Projects/SINOTH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t xml:space="preserve">FSOS_ALL_DISTRIBUTOR_ALL_CAT_ALL_BRAND_ALL_SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FACINGS_COUNT_BY_DISTRIBUTOR_SCENETYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FACINGS_COUNT_BY_DISTRIBUTOR_SCENETYPE_SKU</t>
   </si>
   <si>
     <t xml:space="preserve">kpi_parent</t>
@@ -118,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene_type</t>
   </si>
   <si>
     <t xml:space="preserve">stacking</t>
@@ -193,7 +205,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +256,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFC8F9D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC5F9CB"/>
         <bgColor rgb="FFC8F9D0"/>
       </patternFill>
@@ -257,7 +275,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5C2F5"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -335,7 +353,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -380,6 +398,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -396,10 +426,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -409,6 +435,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,6 +474,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -476,7 +514,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -513,7 +559,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -565,18 +611,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="E9 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,9 +698,30 @@
       </c>
       <c r="D7" s="6"/>
     </row>
+    <row r="8" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -670,72 +738,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:7"/>
+  <dimension ref="1:9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="52.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="11" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="11" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1021" min="15" style="11" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="49.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="14" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="14" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1021" min="15" style="14" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="O1" s="0"/>
       <c r="P1" s="0"/>
@@ -1746,33 +1814,33 @@
       <c r="AMG1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="14" t="s">
+      <c r="C2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="14" t="s">
-        <v>27</v>
+      <c r="H2" s="19"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="O2" s="0"/>
       <c r="P2" s="0"/>
@@ -2786,32 +2854,32 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="14" t="s">
+      <c r="C3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>29</v>
+      <c r="D3" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="O3" s="0"/>
       <c r="P3" s="0"/>
@@ -3825,34 +3893,34 @@
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="C4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="14" t="s">
+      <c r="M4" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="18" t="s">
         <v>27</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>24</v>
       </c>
       <c r="O4" s="0"/>
       <c r="P4" s="0"/>
@@ -4863,35 +4931,35 @@
       <c r="AMG4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>27</v>
+      <c r="N5" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="O5" s="0"/>
       <c r="P5" s="0"/>
@@ -5901,81 +5969,143 @@
       <c r="AMF5" s="0"/>
       <c r="AMG5" s="0"/>
     </row>
-    <row r="6" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+    <row r="6" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="AMH6" s="25"/>
-      <c r="AMI6" s="25"/>
-      <c r="AMJ6" s="25"/>
+      <c r="N6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AMH6" s="28"/>
+      <c r="AMI6" s="28"/>
+      <c r="AMJ6" s="28"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="18" t="s">
+      <c r="N7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AMH7" s="28"/>
+      <c r="AMI7" s="28"/>
+      <c r="AMJ7" s="28"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="30"/>
+      <c r="B8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="14" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30"/>
+      <c r="B9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N7" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="AMH7" s="25"/>
-      <c r="AMI7" s="25"/>
-      <c r="AMJ7" s="25"/>
+      <c r="N9" s="30" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5993,79 +6123,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:8"/>
+  <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F30" activeCellId="1" sqref="E9 F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="28" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="20.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="27" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="32" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="32" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="32" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="33" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="32" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="32" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="32" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="32" width="10.3928571428571"/>
   </cols>
   <sheetData>
-    <row r="1" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+    <row r="1" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="29" t="s">
+      <c r="B1" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="C1" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="D1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="E1" s="35" t="s">
         <v>39</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="33" t="n">
+      <c r="B2" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="33" t="n">
+      <c r="C2" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="33" t="n">
+      <c r="D2" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="33" t="n">
+      <c r="E2" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
+      <c r="F2" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
@@ -7083,162 +7213,214 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="34" t="n">
+      <c r="B3" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="34" t="n">
+      <c r="C3" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="34" t="n">
+      <c r="D3" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="34" t="n">
+      <c r="E3" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
+      <c r="F3" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="34" t="n">
+      <c r="B4" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="34" t="n">
+      <c r="C4" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="34" t="n">
+      <c r="D4" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="34" t="n">
+      <c r="E4" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
+      <c r="F4" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
       <c r="J4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="34" t="n">
+      <c r="B5" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="34" t="n">
+      <c r="C5" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="34" t="n">
+      <c r="D5" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="34" t="n">
+      <c r="E5" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
+      <c r="F5" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="34" t="n">
+      <c r="B6" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="34" t="n">
+      <c r="C6" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="34" t="n">
+      <c r="D6" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="34" t="n">
+      <c r="E6" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
+      <c r="F6" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="34" t="n">
+      <c r="B7" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="34" t="n">
+      <c r="C7" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="34" t="n">
+      <c r="D7" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="34" t="n">
+      <c r="E7" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="F7" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
       <c r="J7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="34" t="n">
+    <row r="8" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="41" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>43</v>
+      <c r="D8" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding scene level KPI
</commit_message>
<xml_diff>
--- a/Projects/SINOTH/Data/Template.xlsx
+++ b/Projects/SINOTH/Data/Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="48">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -57,13 +57,16 @@
     <t xml:space="preserve">FSOS_ALL_DISTRIBUTOR_ALL_CAT_ALL_BRAND_ALL_SKU</t>
   </si>
   <si>
-    <t xml:space="preserve">FACINGS_COUNT_BY_DISTRIBUTOR_SCENETYPE</t>
+    <t xml:space="preserve">FACINGS_COUNT_BY_DISTRIBUTOR_SCENE</t>
   </si>
   <si>
     <t xml:space="preserve">SIMON</t>
   </si>
   <si>
-    <t xml:space="preserve">FACINGS_COUNT_BY_DISTRIBUTOR_SCENETYPE_SKU</t>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FACINGS_COUNT_BY_DISTRIBUTOR_SCENE_SKU</t>
   </si>
   <si>
     <t xml:space="preserve">kpi_parent</t>
@@ -127,9 +130,6 @@
   </si>
   <si>
     <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scene_type</t>
   </si>
   <si>
     <t xml:space="preserve">stacking</t>
@@ -205,7 +205,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +256,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC9B6B6"/>
+        <bgColor rgb="FFC5C2F5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFC8F9D0"/>
       </patternFill>
@@ -275,7 +281,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5C2F5"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFC9B6B6"/>
       </patternFill>
     </fill>
     <fill>
@@ -353,7 +359,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -402,11 +408,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,10 +440,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -439,6 +449,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -474,11 +488,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,7 +540,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -551,7 +577,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFC9B6B6"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -576,7 +602,7 @@
       <rgbColor rgb="FF66FF99"/>
       <rgbColor rgb="FFF69ABE"/>
       <rgbColor rgb="FFFF66CC"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33FF99"/>
       <rgbColor rgb="FF66CC00"/>
@@ -606,17 +632,17 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.0816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,15 +725,15 @@
         <v>12</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>13</v>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -736,67 +762,67 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topRight" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="49.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="14" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="14" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="14" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="14" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="14" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1021" min="15" style="14" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="47.9234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="16" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="16" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="16" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="16" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1021" min="15" style="16" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="15" t="s">
         <v>26</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="O1" s="0"/>
       <c r="P1" s="0"/>
@@ -1807,33 +1833,33 @@
       <c r="AMG1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="18" t="s">
+      <c r="C2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="18" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="L2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>30</v>
+      <c r="M2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="O2" s="0"/>
       <c r="P2" s="0"/>
@@ -2847,32 +2873,32 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>32</v>
+      <c r="N3" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="O3" s="0"/>
       <c r="P3" s="0"/>
@@ -3886,34 +3912,34 @@
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="23"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="18" t="s">
-        <v>27</v>
+      <c r="N4" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="O4" s="0"/>
       <c r="P4" s="0"/>
@@ -4924,35 +4950,35 @@
       <c r="AMG4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16"/>
-      <c r="B5" s="25" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="18" t="s">
+      <c r="C5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="18" t="s">
+      <c r="D5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="22" t="s">
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="19" t="s">
         <v>31</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>30</v>
       </c>
       <c r="O5" s="0"/>
       <c r="P5" s="0"/>
@@ -5962,142 +5988,138 @@
       <c r="AMF5" s="0"/>
       <c r="AMG5" s="0"/>
     </row>
-    <row r="6" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
+    <row r="6" s="29" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="20" t="s">
+      <c r="C6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="AMH6" s="28"/>
-      <c r="AMI6" s="28"/>
-      <c r="AMJ6" s="28"/>
+      <c r="N6" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AMH6" s="30"/>
+      <c r="AMI6" s="30"/>
+      <c r="AMJ6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="AMH7" s="28"/>
-      <c r="AMI7" s="28"/>
-      <c r="AMJ7" s="28"/>
+      <c r="N7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AMH7" s="30"/>
+      <c r="AMI7" s="30"/>
+      <c r="AMJ7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="22" t="s">
+      <c r="C8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="31" t="s">
-        <v>30</v>
+      <c r="M8" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30"/>
-      <c r="B9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="22" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="N9" s="30" t="s">
-        <v>33</v>
+      <c r="M9" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -6119,76 +6141,76 @@
   <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="32" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="32" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="32" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="33" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="32" width="34.3622448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="32" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="32" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="32" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="55.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="36" width="8.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="6.87755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="9.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="6.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="37" width="22.1632653061224"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="34.3622448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="36" width="17.3775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="36" width="20.9234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="36" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+    <row r="1" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="40" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="38" t="n">
+      <c r="B2" s="42" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="38" t="n">
+      <c r="C2" s="42" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="38" t="n">
+      <c r="D2" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="42" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
@@ -7206,192 +7228,192 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="39" t="n">
+      <c r="B3" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="39" t="n">
+      <c r="C3" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="39" t="n">
+      <c r="D3" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="39" t="n">
+      <c r="B4" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="39" t="n">
+      <c r="C4" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="39" t="n">
+      <c r="D4" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
       <c r="J4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="39" t="n">
+      <c r="B5" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="39" t="n">
+      <c r="C5" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="39" t="n">
+      <c r="D5" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="39" t="n">
+      <c r="B6" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="39" t="n">
+      <c r="C6" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="39" t="n">
+      <c r="D6" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="39" t="n">
+      <c r="B7" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="39" t="n">
+      <c r="C7" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="39" t="n">
+      <c r="D7" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="43" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
       <c r="J7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="40" t="n">
+      <c r="C8" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="40" t="n">
+      <c r="D8" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
       <c r="J8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="40" t="n">
+      <c r="A9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="40" t="n">
+      <c r="C9" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="40" t="n">
+      <c r="D9" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="39" t="n">
+      <c r="B10" s="43" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -7400,13 +7422,13 @@
       <c r="D10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="42" t="s">
         <v>45</v>
       </c>
       <c r="H10" s="4" t="s">

</xml_diff>

<commit_message>
adding promotional shelf for simon kpi
</commit_message>
<xml_diff>
--- a/Projects/SINOTH/Data/Template.xlsx
+++ b/Projects/SINOTH/Data/Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t xml:space="preserve">candy, chocolate, gum, gummy, lollipop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Shelf, Promotional Shelf</t>
   </si>
   <si>
     <t xml:space="preserve">ASSORTMENTS</t>
@@ -637,12 +640,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,18 +770,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="47.9234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="16" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="16" width="12.7448979591837"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="16" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="16" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1021" min="15" style="16" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="16" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="16" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="16" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="16" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1021" min="15" style="16" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6141,21 +6144,21 @@
   <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="55.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="36" width="8.5765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="6.87755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="9.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="6.72448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="37" width="22.1632653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="34.3622448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="36" width="17.3775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="36" width="20.9234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="36" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="36" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="37" width="26.484693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="36" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="36" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="36" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7374,7 +7377,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G8" s="34" t="s">
         <v>45</v>
@@ -7399,10 +7402,10 @@
       <c r="E9" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="42" t="s">
+      <c r="F9" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="45" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="45"/>
@@ -7411,19 +7414,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="43" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" s="47" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F10" s="42" t="s">
         <v>44</v>
@@ -7432,10 +7435,10 @@
         <v>45</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excluded empty and irrelevant
</commit_message>
<xml_diff>
--- a/Projects/SINOTH/Data/Template.xlsx
+++ b/Projects/SINOTH/Data/Template.xlsx
@@ -635,18 +635,17 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="G10 A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,23 +765,23 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K21" activeCellId="1" sqref="G10 K21"/>
+      <selection pane="topRight" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="52.5102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="16" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="16" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="16" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="16" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1021" min="15" style="16" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="51.969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="16" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="16" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="16" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="16" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1021" min="15" style="16" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="6.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6145,21 +6144,21 @@
   <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="53.1887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="36" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="37" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="42.0816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="36" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="36" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="36" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="52.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="36" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="37" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="36" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="36" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="36" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6202,7 +6201,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="42" t="n">
         <v>0</v>
@@ -7242,7 +7241,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="43" t="n">
         <v>0</v>
@@ -7268,7 +7267,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="43" t="n">
         <v>0</v>
@@ -7294,7 +7293,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="43" t="n">
         <v>0</v>
@@ -7320,7 +7319,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="43" t="n">
         <v>0</v>
@@ -7346,7 +7345,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="43" t="n">
         <v>0</v>
@@ -7372,7 +7371,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="44" t="n">
         <v>0</v>
@@ -7398,7 +7397,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="45" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
removed general, updated tests
</commit_message>
<xml_diff>
--- a/Projects/SINOTH/Data/Template.xlsx
+++ b/Projects/SINOTH/Data/Template.xlsx
@@ -159,7 +159,7 @@
     <t xml:space="preserve">Main Shelf</t>
   </si>
   <si>
-    <t xml:space="preserve">General, candy, chocolate, gum, gummy, lollipop</t>
+    <t xml:space="preserve">candy, chocolate, gum, gummy, lollipop</t>
   </si>
   <si>
     <t xml:space="preserve">Main Shelf, Promotional Shelf</t>
@@ -640,12 +640,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.1887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,18 +769,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="45.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="51.969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="16" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="16" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="16" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="16" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1021" min="15" style="16" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="44.9540816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="16" width="6.75"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="16" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="16" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="16" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1021" min="15" style="16" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6149,16 +6148,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="52.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="36" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="37" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="36" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="36" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="36" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="51.969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="36" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="37" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="36" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="36" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="36" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>